<commit_message>
Update PPR and brucellosis AHLE parameter files
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/PPR_AHLE scenario parameters SMALLRUMINANTS_20230329.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/PPR_AHLE scenario parameters SMALLRUMINANTS_20230329.xlsx
@@ -1069,22 +1069,22 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>rgamma(10000,9.73797721710479,11.0282601519232)</t>
+          <t>rgamma(10000,9.8731995367749,11.2128609319927)</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>rgamma(10000,45.8116722726295,56.9664546211285)</t>
+          <t>rgamma(10000,45.545556222724,56.8170215196901)</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>rgamma(10000,19.1153348661887,23.6746083740052)</t>
+          <t>rgamma(10000,19.021394202597,23.6288060522362)</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>rgamma(10000,60.0543543752376,71.1090177392434)</t>
+          <t>rgamma(10000,61.0324282301941,72.345654204045)</t>
         </is>
       </c>
     </row>
@@ -1600,12 +1600,29 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>8.1666666666666665E-2</t>
+        </is>
+      </c>
+    </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
           <t># Mortality ## informed from META analysis</t>
         </is>
       </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>1.4999999999999999E-2</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>3.3333333333333333E-2</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1660,22 +1677,22 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>rgamma(10000,2.92884715065396,1561.05714669918)</t>
+          <t>rgamma(10000,3.61170067257074,3403.43585425309)</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>rgamma(10000,2.95035960085304,1677.44420933577)</t>
+          <t>rgamma(10000,3.60960309269834,3234.05400729713)</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>rgamma(10000,2.67516706420522,447.071064786197)</t>
+          <t>rgamma(10000,2.89973650608414,1382.80543309279)</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>rgamma(10000,2.7644413784333,714.555635978384)</t>
+          <t>rgamma(10000,2.96996945220457,1352.89487200589)</t>
         </is>
       </c>
     </row>
@@ -1732,22 +1749,22 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.33480622490792,1577.56186402102)</t>
+          <t>rgamma(10000,4.21154853218239,3539.49622589056)</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.36787569022991,1693.26600657936)</t>
+          <t>rgamma(10000,4.19063547534716,3306.6993145909)</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>rgamma(10000,2.89263038799833,471.142351557217)</t>
+          <t>rgamma(10000,3.15274454073964,1465.75890925845)</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>rgamma(10000,2.87778750457611,733.027543666483)</t>
+          <t>rgamma(10000,3.16041418729247,1413.90407390784)</t>
         </is>
       </c>
     </row>
@@ -1804,22 +1821,22 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.47959163317464,1773.50207639399)</t>
+          <t>rgamma(10000,4.44815194346767,4002.40107198309)</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.46734874424675,1850.25101268803)</t>
+          <t>rgamma(10000,4.60386165488748,3894.74739558975)</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.15452188367403,503.493205746653)</t>
+          <t>rgamma(10000,3.4930659319298,1602.88553751651)</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.1530900641198,788.083617976066)</t>
+          <t>rgamma(10000,3.54212155682475,1564.95658431496)</t>
         </is>
       </c>
     </row>
@@ -1876,22 +1893,22 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.48179800831633,1756.81034111698)</t>
+          <t>rgamma(10000,4.46975086236396,4042.30975498851)</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.50615670077232,1894.23585567003)</t>
+          <t>rgamma(10000,4.60818773709151,3904.21069711548)</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.13766535029488,501.690030124566)</t>
+          <t>rgamma(10000,3.49084487076966,1613.46183712223)</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.06973416832905,771.265992191836)</t>
+          <t>rgamma(10000,3.46785111439653,1526.74941595658)</t>
         </is>
       </c>
     </row>
@@ -4579,22 +4596,22 @@
       </c>
       <c r="K115" t="inlineStr">
         <is>
-          <t>rgamma(10000,5.15380360784384,99.6770855721607)</t>
+          <t>rgamma(10000,7.93941338084862,272.859442324841)</t>
         </is>
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>rgamma(10000,5.12447589499906,105.026050355092)</t>
+          <t>rgamma(10000,7.76882162737506,250.445061203992)</t>
         </is>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>rgamma(10000,7.12544210325944,69.4626439243428)</t>
+          <t>rgamma(10000,9.19838639987883,256.467213555895)</t>
         </is>
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>rgamma(10000,7.0351657144291,107.313635083522)</t>
+          <t>rgamma(10000,9.22030903876569,247.35385289858)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update PPR and Brucellosis scenarios for small ruminants
Rerun disease models as Wudu provided new current and ideal parameters.
</commit_message>
<xml_diff>
--- a/Ethiopia Workspace/Code and Control Files/PPR_AHLE scenario parameters SMALLRUMINANTS_20230329.xlsx
+++ b/Ethiopia Workspace/Code and Control Files/PPR_AHLE scenario parameters SMALLRUMINANTS_20230329.xlsx
@@ -1029,17 +1029,17 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>rpert(10000, 0.3, 1.8, 0.8)</t>
+          <t>rpert(10000, 0.52, 1.8, 0.8)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>rpert(10000, 0.25, 1.2, 0.85)</t>
+          <t>rpert(10000, 0.37, 1.2, 0.85)</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>rpert(10000, 0.5, 1.12, 0.80)</t>
+          <t>rpert(10000, 0.52, 1.12, 0.80)</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1069,22 +1069,22 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>rgamma(10000,9.8731995367749,11.2128609319927)</t>
+          <t>rgamma(10000,17.4466432134836,18.9776334167698)</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>rgamma(10000,45.545556222724,56.8170215196901)</t>
+          <t>rgamma(10000,49.3999046519414,61.3693584882142)</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>rgamma(10000,19.021394202597,23.6288060522362)</t>
+          <t>rgamma(10000,27.0092026904415,32.700265012487)</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>rgamma(10000,61.0324282301941,72.345654204045)</t>
+          <t>rgamma(10000,60.4640687388793,71.6207865781374)</t>
         </is>
       </c>
     </row>
@@ -1116,22 +1116,22 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>rtruncnorm(10000, 0, 3, 1.3, 0.15)</t>
+          <t>rtruncnorm(10000,1 3, 1.3, 0.15)</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>rtruncnorm(10000, a = 0, b = 3, 1.7, 0.12)</t>
+          <t>rtruncnorm(10000, a = 1, b = 3, 1.7, 0.12)</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>rtruncnorm(10000, 0, 3, 1.3, 0.25)</t>
+          <t>rtruncnorm(10000, 1, 3, 1.3, 0.25)</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>rtruncnorm(10000, 0, 3, 1.7, 0.12)</t>
+          <t>rtruncnorm(10000, 1, 3, 1.7, 0.12)</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.06</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1185,7 +1185,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.19</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1195,7 +1195,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.06</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.19</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1220,12 +1220,12 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.06</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.19</t>
         </is>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>129</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>117</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1267,7 +1267,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>129</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>117</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1292,12 +1292,12 @@
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>129</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>117</t>
         </is>
       </c>
     </row>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.53</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.44</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.53</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1344,7 +1344,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.44</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1359,12 +1359,12 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>rgamma(10000,3772368.57000284,7128389.1044237)</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>rgamma(10000,3793791.32733981,8635195.85357711)</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>40</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>40</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>40</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>40</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1426,10 +1426,27 @@
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>40</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1600,29 +1617,12 @@
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>8.1666666666666665E-2</t>
-        </is>
-      </c>
-    </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
           <t># Mortality ## informed from META analysis</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>1.4999999999999999E-2</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>3.3333333333333333E-2</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1682,17 +1682,17 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.60960309269834,3234.05400729713)</t>
+          <t>rgamma(10000,3.61714833585507,3247.99695514058)</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>rgamma(10000,2.89973650608414,1382.80543309279)</t>
+          <t>rgamma(10000,2.90990208584108,1392.05710182917)</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>rgamma(10000,2.96996945220457,1352.89487200589)</t>
+          <t>rgamma(10000,2.95346605196759,1347.79254054126)</t>
         </is>
       </c>
     </row>
@@ -1739,7 +1739,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>rpert(1000, 0.05/6, 0.05/6, 0.05/6)</t>
+          <t>rpert(1000, 0.03/6, 0.30/6, 0.07/6)</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -1754,17 +1754,17 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>rgamma(10000,4.19063547534716,3306.6993145909)</t>
+          <t>rgamma(10000,4.21831343905007,3327.33480810473)</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.15274454073964,1465.75890925845)</t>
+          <t>rgamma(10000,3.19100794226407,1485.53080973414)</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.16041418729247,1413.90407390784)</t>
+          <t>rgamma(10000,3.30436860091543,1482.27033519595)</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>rpert(1000, 0.04/12, 0.04/12, 0.04/12)</t>
+          <t>rpert(1000, 0.02/12, 0.13/12, 0.05/12)</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -1826,17 +1826,17 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>rgamma(10000,4.60386165488748,3894.74739558975)</t>
+          <t>rgamma(10000,4.5008332239152,3800.98013960957)</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.4930659319298,1602.88553751651)</t>
+          <t>rgamma(10000,3.50406942954506,1608.06250528434)</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.54212155682475,1564.95658431496)</t>
+          <t>rgamma(10000,3.50174516903281,1545.59116876794)</t>
         </is>
       </c>
     </row>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>rpert(1000, 0.05/12, 0.05/12, 0.05/12)</t>
+          <t>rpert(1000, 0.02/12, 0.17/12, 0.06/12)</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -1898,17 +1898,17 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>rgamma(10000,4.60818773709151,3904.21069711548)</t>
+          <t>rgamma(10000,4.57000263641882,3866.79894366496)</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.49084487076966,1613.46183712223)</t>
+          <t>rgamma(10000,3.49179451164479,1613.37195080481)</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>rgamma(10000,3.46785111439653,1526.74941595658)</t>
+          <t>rgamma(10000,3.50637017037747,1543.86070529131)</t>
         </is>
       </c>
     </row>
@@ -2090,7 +2090,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>rpert(10000, 6, 23, 12.6 )</t>
+          <t>rpert(10000, 7.3, 23, 12.6 )</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -2100,12 +2100,12 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>rpert(10000, 6.5, 16.5, 14 )</t>
+          <t>rpert(10000, 7.3, 16.5, 14 )</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>rpert(10000, 6, 15.5, 13 )</t>
+          <t>rpert(10000, 6.2, 15.5, 13 )</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2130,12 +2130,12 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>rpert(10000, 6, 23, 12.6 )</t>
+          <t>rpert(10000, 7.3, 23, 12.6 )</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>rpert(10000, 6.5, 16.5, 14 )</t>
+          <t>rpert(10000, 7.3, 16.5, 14 )</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
@@ -2145,7 +2145,7 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>rpert(10000, 6, 15.5, 13 )</t>
+          <t>rpert(10000, 6.2, 15.5, 13 )</t>
         </is>
       </c>
     </row>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>rpert(10000, 7, 17.0, 13.8)</t>
+          <t>rpert(10000, 7.3, 17.0, 13.8)</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2207,7 +2207,7 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>rpert(10000, 7, 17.0, 13.8)</t>
+          <t>rpert(10000, 7.3, 17.0, 13.8)</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
@@ -2234,17 +2234,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>rpert(10000, 11, 30, 21.5)</t>
+          <t>rpert(10000, 13.5, 30, 21.5)</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>rpert(10000, 10, 30, 21.0)</t>
+          <t>rpert(10000, 11.6, 30, 21.0)</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>rpert(10000, 12, 23, 17.4)</t>
+          <t>rnorm(10000, 19.1, sd = 0.48)</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2274,17 +2274,17 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>rpert(10000, 11, 30, 21.5)</t>
+          <t>rpert(10000, 13.5, 30, 21.5)</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>rpert(10000, 12, 23, 17.4)</t>
+          <t>rnorm(10000, 19.1, sd = 0.48)</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>rpert(10000, 10, 30, 21.0)</t>
+          <t>rpert(10000, 11.6, 30, 21.0)</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
@@ -2316,7 +2316,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>rpert(10000, 12.5, 24, 18)</t>
+          <t>rnorm(10000, 19.1, sd = 0.48)</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>rpert(10000, 12.5, 24, 18)</t>
+          <t>rnorm(10000, 19.1, sd = 0.48)</t>
         </is>
       </c>
       <c r="M46" t="inlineStr">
@@ -2378,22 +2378,22 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>rpert(10000, 18, 38, 31.2 )</t>
+          <t>rpert(10000, 20.4, 38, 31.2 )</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>rpert(10000, 16, 35, 28.2 )</t>
+          <t>rpert(10000, 24.7, 35, 28.2 )</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>rpert(10000, 17, 34, 29.0)</t>
+          <t>rnorm(10000, 29.6, sd = 0.7)</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>rpert(10000, 15, 33, 27.5)</t>
+          <t>rpert(10000, 24.7, 33, 27.5)</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2418,22 +2418,22 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>rpert(10000, 18, 38, 31.2 )</t>
+          <t>rpert(10000, 20.4, 38, 31.2 )</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>rpert(10000, 17, 34, 29.0)</t>
+          <t>rnorm(10000, 29.6, sd = 0.7)</t>
         </is>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>rpert(10000, 16, 35, 28.2 )</t>
+          <t>rpert(10000, 24.7, 35, 28.2 )</t>
         </is>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>rpert(10000, 15, 33, 27.5)</t>
+          <t>rpert(10000, 24.7, 33, 27.5)</t>
         </is>
       </c>
     </row>
@@ -2450,22 +2450,22 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>rpert(10000, 20, 45, 34.3)</t>
+          <t>rpert(10000, 20, 45.1, 34.3)</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>rpert(10000, 18, 37, 30.7)</t>
+          <t>rpert(10000, 23.7, 37, 30.7)</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>rpert(10000, 18, 40.5, 30)</t>
+          <t>rnorm(10000, 31.5, sd = 6.8)</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>rpert(10000, 17, 45, 29)</t>
+          <t>rpert(10000, 24.7, 45, 29)</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2490,22 +2490,22 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>rpert(10000, 20, 45, 34.3)</t>
+          <t>rpert(10000, 20, 45.1, 34.3)</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>rpert(10000, 18, 40.5, 30)</t>
+          <t>rnorm(10000, 31.5, sd = 6.8)</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>rpert(10000, 18, 37, 30.7)</t>
+          <t>rpert(10000, 23.7, 37, 30.7)</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>rpert(10000, 17, 45, 29)</t>
+          <t>rpert(10000, 24.7, 45, 29)</t>
         </is>
       </c>
     </row>
@@ -4601,17 +4601,17 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>rgamma(10000,7.76882162737506,250.445061203992)</t>
+          <t>rgamma(10000,7.86174175298633,253.37192569172)</t>
         </is>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>rgamma(10000,9.19838639987883,256.467213555895)</t>
+          <t>rgamma(10000,9.34440461900789,260.880417477159)</t>
         </is>
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>rgamma(10000,9.22030903876569,247.35385289858)</t>
+          <t>rgamma(10000,9.27074476872806,250.339966707991)</t>
         </is>
       </c>
     </row>

</xml_diff>